<commit_message>
payment page without UI
</commit_message>
<xml_diff>
--- a/Project Detail/DataDic.xlsx
+++ b/Project Detail/DataDic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gotj\Desktop\WebProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gotj\Desktop\WebProject\Project Detail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF65B01-EF8F-480D-8CBD-611B91D18DD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BAD38D-B0C2-4C9E-A083-B47EDEBCCEB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="1350" windowWidth="24750" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="แผ่น1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="110">
   <si>
     <t>No.</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t>รูปใบเสร็จ</t>
+  </si>
+  <si>
+    <t>RoomImage</t>
+  </si>
+  <si>
+    <t>Img</t>
+  </si>
+  <si>
+    <t>รูปตัวอย่างห้อง</t>
   </si>
 </sst>
 </file>
@@ -714,10 +723,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1548,6 +1557,26 @@
         <v>103</v>
       </c>
     </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>